<commit_message>
Support snirf and nirs
Data format and 2d project to support snirf and nirs data format
</commit_message>
<xml_diff>
--- a/NIRSmat_structureinformation.xlsx
+++ b/NIRSmat_structureinformation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="408">
   <si>
     <t>Appareil</t>
   </si>
@@ -705,9 +705,6 @@
     <t>Sampling frequency</t>
   </si>
   <si>
-    <t>(a voir!!!!!!!!!!!)</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -1072,9 +1069,6 @@
   </si>
   <si>
     <t>P situated in ROI</t>
-  </si>
-  <si>
-    <t>!!!!!!!! A SUPPRIMER, NON ??</t>
   </si>
   <si>
     <t>possiblités de confusion avec les vraies longueurs d'ondes utilisées dans les channels</t>
@@ -1818,7 +1812,7 @@
   <dimension ref="A1:AJ174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I164" sqref="I164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,13 +1871,13 @@
     </row>
     <row r="2" spans="1:36" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="K2" s="24" t="s">
         <v>336</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>338</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -1976,11 +1970,9 @@
       <c r="C6" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="27" t="s">
-        <v>351</v>
-      </c>
+      <c r="D6" s="27"/>
       <c r="E6" s="42" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
@@ -2068,9 +2060,7 @@
       <c r="C8" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="D8" s="34" t="s">
-        <v>228</v>
-      </c>
+      <c r="D8" s="34"/>
       <c r="E8" s="34"/>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
@@ -2244,7 +2234,7 @@
       <c r="A12" s="37"/>
       <c r="B12" s="25"/>
       <c r="C12" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -2256,7 +2246,7 @@
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L12" s="17"/>
       <c r="M12" s="1"/>
@@ -2302,7 +2292,7 @@
         <v>55</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L13" s="18"/>
       <c r="M13" s="1"/>
@@ -2348,7 +2338,7 @@
         <v>28</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L14" s="18"/>
       <c r="M14" s="1"/>
@@ -2392,7 +2382,7 @@
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L15" s="18"/>
       <c r="M15" s="1"/>
@@ -2436,7 +2426,7 @@
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L16" s="18"/>
       <c r="M16" s="1"/>
@@ -2480,7 +2470,7 @@
         <v>36</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L17" s="18"/>
       <c r="M17" s="1"/>
@@ -2526,7 +2516,7 @@
         <v>41</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L18" s="18"/>
       <c r="M18" s="1"/>
@@ -2570,7 +2560,7 @@
         <v>45</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="1"/>
@@ -2614,7 +2604,7 @@
         <v>46</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L20" s="18"/>
       <c r="M20" s="1"/>
@@ -2658,7 +2648,7 @@
       </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L21" s="18"/>
       <c r="M21" s="1"/>
@@ -2702,7 +2692,7 @@
         <v>37</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L22" s="18"/>
       <c r="M22" s="1"/>
@@ -2750,7 +2740,7 @@
         <v>42</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L23" s="18"/>
       <c r="M23" s="1"/>
@@ -2796,7 +2786,7 @@
         <v>43</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L24" s="18"/>
       <c r="M24" s="1"/>
@@ -2835,16 +2825,16 @@
         <v>3</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I25" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="J25" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="K25" s="9" t="s">
         <v>300</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>301</v>
       </c>
       <c r="L25" s="18"/>
       <c r="M25" s="1"/>
@@ -2888,7 +2878,7 @@
         <v>44</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L26" s="18"/>
       <c r="M26" s="1"/>
@@ -2927,16 +2917,16 @@
         <v>3</v>
       </c>
       <c r="H27" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I27" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="J27" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>282</v>
-      </c>
       <c r="K27" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L27" s="18"/>
       <c r="M27" s="1"/>
@@ -2970,7 +2960,7 @@
       <c r="C28" s="15"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>14</v>
@@ -2982,7 +2972,7 @@
         <v>48</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L28" s="18"/>
       <c r="M28" s="1"/>
@@ -3026,7 +3016,7 @@
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L29" s="18"/>
       <c r="M29" s="1"/>
@@ -3070,7 +3060,7 @@
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L30" s="18"/>
       <c r="M30" s="1"/>
@@ -3114,7 +3104,7 @@
         <v>50</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L31" s="18"/>
       <c r="M31" s="1"/>
@@ -3162,7 +3152,7 @@
         <v>51</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L32" s="18"/>
       <c r="M32" s="1"/>
@@ -3206,7 +3196,7 @@
         <v>53</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L33" s="18"/>
       <c r="M33" s="1"/>
@@ -3242,7 +3232,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H34" s="8" t="s">
         <v>17</v>
@@ -3254,7 +3244,7 @@
         <v>54</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L34" s="18"/>
       <c r="M34" s="1"/>
@@ -3385,10 +3375,10 @@
       </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L37" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -3431,10 +3421,10 @@
         <v>36</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
@@ -3473,16 +3463,16 @@
       </c>
       <c r="H39" s="8"/>
       <c r="I39" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J39" s="9" t="s">
         <v>41</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
@@ -3528,7 +3518,7 @@
         <v>146</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
@@ -3574,7 +3564,7 @@
         <v>147</v>
       </c>
       <c r="L41" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
@@ -3624,7 +3614,7 @@
         <v>221</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
@@ -3670,7 +3660,7 @@
         <v>220</v>
       </c>
       <c r="L43" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
@@ -3716,7 +3706,7 @@
         <v>219</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
@@ -3762,7 +3752,7 @@
         <v>148</v>
       </c>
       <c r="L45" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
@@ -3812,7 +3802,7 @@
         <v>218</v>
       </c>
       <c r="L46" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
@@ -4340,20 +4330,20 @@
       <c r="B58" s="7"/>
       <c r="C58" s="15"/>
       <c r="D58" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E58" s="39"/>
       <c r="F58" s="39"/>
       <c r="G58" s="39"/>
       <c r="H58" s="9"/>
       <c r="I58" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J58" s="9" t="s">
         <v>91</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L58" s="10"/>
       <c r="M58" s="1"/>
@@ -4571,11 +4561,11 @@
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J63" s="5"/>
       <c r="K63" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L63" s="6"/>
       <c r="M63" s="1"/>
@@ -4618,10 +4608,10 @@
         <v>55</v>
       </c>
       <c r="J64" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="K64" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="K64" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="L64" s="18"/>
       <c r="M64" s="1"/>
@@ -4664,10 +4654,10 @@
         <v>28</v>
       </c>
       <c r="J65" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="K65" s="9" t="s">
         <v>233</v>
-      </c>
-      <c r="K65" s="9" t="s">
-        <v>234</v>
       </c>
       <c r="L65" s="10"/>
       <c r="M65" s="1"/>
@@ -4700,20 +4690,20 @@
       <c r="B66" s="7"/>
       <c r="C66" s="15"/>
       <c r="D66" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E66" s="39"/>
       <c r="F66" s="39"/>
       <c r="G66" s="39"/>
       <c r="H66" s="9"/>
       <c r="I66" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J66" s="9" t="s">
         <v>91</v>
       </c>
       <c r="K66" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L66" s="10"/>
       <c r="M66" s="1"/>
@@ -4757,7 +4747,7 @@
       </c>
       <c r="J67" s="8"/>
       <c r="K67" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L67" s="18"/>
       <c r="M67" s="1"/>
@@ -4801,7 +4791,7 @@
       </c>
       <c r="J68" s="8"/>
       <c r="K68" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L68" s="18"/>
       <c r="M68" s="1"/>
@@ -4845,7 +4835,7 @@
         <v>36</v>
       </c>
       <c r="K69" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L69" s="18"/>
       <c r="M69" s="1"/>
@@ -4885,13 +4875,13 @@
       </c>
       <c r="H70" s="9"/>
       <c r="I70" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J70" s="9" t="s">
         <v>41</v>
       </c>
       <c r="K70" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L70" s="18"/>
       <c r="M70" s="1"/>
@@ -4923,7 +4913,7 @@
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -5274,7 +5264,7 @@
       <c r="B79" s="7"/>
       <c r="C79" s="15"/>
       <c r="D79" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
@@ -5283,7 +5273,7 @@
       <c r="I79" s="9"/>
       <c r="J79" s="9"/>
       <c r="K79" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L79" s="10"/>
       <c r="M79" s="1"/>
@@ -5500,20 +5490,20 @@
       <c r="B84" s="7"/>
       <c r="C84" s="15"/>
       <c r="D84" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
       <c r="H84" s="9"/>
       <c r="I84" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="J84" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="J84" s="9" t="s">
+      <c r="K84" s="9" t="s">
         <v>252</v>
-      </c>
-      <c r="K84" s="9" t="s">
-        <v>253</v>
       </c>
       <c r="L84" s="10"/>
       <c r="M84" s="1"/>
@@ -5674,7 +5664,7 @@
         <v>149</v>
       </c>
       <c r="L88" s="43" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
@@ -5718,7 +5708,7 @@
         <v>150</v>
       </c>
       <c r="L89" s="44" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
@@ -5762,7 +5752,7 @@
         <v>151</v>
       </c>
       <c r="L90" s="44" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
@@ -5836,7 +5826,7 @@
     <row r="92" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
       <c r="B92" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
@@ -5848,7 +5838,7 @@
       </c>
       <c r="J92" s="8"/>
       <c r="K92" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L92" s="10"/>
       <c r="M92" s="1"/>
@@ -5879,7 +5869,7 @@
     <row r="93" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
       <c r="B93" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
@@ -5888,11 +5878,11 @@
       <c r="G93" s="8"/>
       <c r="H93" s="8"/>
       <c r="I93" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J93" s="8"/>
       <c r="K93" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L93" s="10"/>
       <c r="M93" s="1"/>
@@ -5924,10 +5914,10 @@
       <c r="A94" s="7"/>
       <c r="B94" s="8"/>
       <c r="C94" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I94" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L94" s="11"/>
       <c r="M94" s="1"/>
@@ -5959,7 +5949,7 @@
       <c r="A95" s="7"/>
       <c r="B95" s="8"/>
       <c r="C95" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D95" s="8"/>
       <c r="E95" s="9"/>
@@ -5971,7 +5961,7 @@
       </c>
       <c r="J95" s="9"/>
       <c r="K95" s="9" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L95" s="11"/>
       <c r="M95" s="1"/>
@@ -6003,7 +5993,7 @@
       <c r="A96" s="7"/>
       <c r="B96" s="8"/>
       <c r="C96" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D96" s="8"/>
       <c r="E96" s="9"/>
@@ -6015,7 +6005,7 @@
       </c>
       <c r="J96" s="8"/>
       <c r="K96" s="9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="L96" s="11"/>
       <c r="M96" s="1"/>
@@ -6059,7 +6049,7 @@
       </c>
       <c r="J97" s="9"/>
       <c r="K97" s="9" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L97" s="11"/>
       <c r="M97" s="1"/>
@@ -6091,7 +6081,7 @@
       <c r="A98" s="7"/>
       <c r="B98" s="8"/>
       <c r="C98" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="9"/>
@@ -6099,11 +6089,11 @@
       <c r="G98" s="9"/>
       <c r="H98" s="9"/>
       <c r="I98" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J98" s="9"/>
       <c r="K98" s="9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L98" s="11"/>
       <c r="M98" s="1"/>
@@ -6135,13 +6125,13 @@
       <c r="A99" s="7"/>
       <c r="B99" s="8"/>
       <c r="C99" t="s">
+        <v>296</v>
+      </c>
+      <c r="I99" t="s">
         <v>297</v>
       </c>
-      <c r="I99" t="s">
-        <v>298</v>
-      </c>
       <c r="K99" s="9" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="L99" s="11"/>
       <c r="M99" s="1"/>
@@ -6173,7 +6163,7 @@
       <c r="A100" s="7"/>
       <c r="B100" s="8"/>
       <c r="C100" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D100" s="8"/>
       <c r="E100" s="8"/>
@@ -6181,11 +6171,11 @@
       <c r="G100" s="8"/>
       <c r="H100" s="8"/>
       <c r="I100" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J100" s="8"/>
       <c r="K100" s="8" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L100" s="11"/>
       <c r="M100" s="1"/>
@@ -6217,7 +6207,7 @@
       <c r="A101" s="7"/>
       <c r="B101" s="8"/>
       <c r="C101" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D101" s="8"/>
       <c r="E101" s="8"/>
@@ -6259,7 +6249,7 @@
       <c r="A102" s="7"/>
       <c r="B102" s="8"/>
       <c r="C102" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D102" s="8"/>
       <c r="E102" s="8"/>
@@ -6271,7 +6261,7 @@
       </c>
       <c r="J102" s="8"/>
       <c r="K102" s="9" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="L102" s="11"/>
       <c r="M102" s="1"/>
@@ -6311,7 +6301,7 @@
       <c r="I103" s="8"/>
       <c r="J103" s="8"/>
       <c r="K103" s="9" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="L103" s="11"/>
       <c r="M103" s="1"/>
@@ -6351,7 +6341,7 @@
       <c r="I104" s="8"/>
       <c r="J104" s="8"/>
       <c r="K104" s="9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="L104" s="11"/>
       <c r="M104" s="1"/>
@@ -6391,7 +6381,7 @@
       <c r="I105" s="8"/>
       <c r="J105" s="8"/>
       <c r="K105" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L105" s="11"/>
       <c r="M105" s="1"/>
@@ -6431,7 +6421,7 @@
       <c r="I106" s="8"/>
       <c r="J106" s="8"/>
       <c r="K106" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="L106" s="11"/>
       <c r="M106" s="1"/>
@@ -6471,7 +6461,7 @@
       <c r="I107" s="8"/>
       <c r="J107" s="8"/>
       <c r="K107" s="9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L107" s="11"/>
       <c r="M107" s="1"/>
@@ -6511,7 +6501,7 @@
       <c r="I108" s="8"/>
       <c r="J108" s="8"/>
       <c r="K108" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L108" s="11"/>
       <c r="M108" s="1"/>
@@ -6550,7 +6540,7 @@
       <c r="I109" s="8"/>
       <c r="J109" s="8"/>
       <c r="K109" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L109" s="11"/>
       <c r="M109" s="1"/>
@@ -6580,7 +6570,7 @@
     </row>
     <row r="110" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A110" s="16" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -6590,11 +6580,11 @@
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
       <c r="I110" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J110" s="4"/>
       <c r="K110" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="L110" s="36"/>
       <c r="M110" s="1"/>
@@ -6625,7 +6615,7 @@
     <row r="111" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A111" s="15"/>
       <c r="B111" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
@@ -6637,7 +6627,7 @@
       </c>
       <c r="J111" s="8"/>
       <c r="K111" s="8" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L111" s="11"/>
       <c r="M111" s="1"/>
@@ -6668,10 +6658,10 @@
     <row r="112" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A112" s="15"/>
       <c r="B112" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D112" s="8"/>
       <c r="E112" s="8"/>
@@ -6679,11 +6669,11 @@
       <c r="G112" s="8"/>
       <c r="H112" s="8"/>
       <c r="I112" s="8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J112" s="8"/>
       <c r="K112" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="L112" s="11"/>
       <c r="M112" s="1"/>
@@ -6715,7 +6705,7 @@
       <c r="A113" s="15"/>
       <c r="B113" s="8"/>
       <c r="C113" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D113" s="8"/>
       <c r="E113" s="9"/>
@@ -6727,7 +6717,7 @@
       </c>
       <c r="J113" s="9"/>
       <c r="K113" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L113" s="11"/>
       <c r="M113" s="1"/>
@@ -6759,13 +6749,13 @@
       <c r="A114" s="15"/>
       <c r="B114" s="8"/>
       <c r="C114" s="9" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I114" t="s">
         <v>96</v>
       </c>
       <c r="K114" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L114" s="11"/>
       <c r="M114" s="1"/>
@@ -6797,13 +6787,13 @@
       <c r="A115" s="15"/>
       <c r="B115" s="8"/>
       <c r="C115" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I115" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K115" s="9" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L115" s="11"/>
       <c r="M115" s="1"/>
@@ -6835,7 +6825,7 @@
       <c r="A116" s="15"/>
       <c r="B116" s="8"/>
       <c r="C116" s="9" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D116" s="8"/>
       <c r="E116" s="9"/>
@@ -6843,11 +6833,11 @@
       <c r="G116" s="9"/>
       <c r="H116" s="9"/>
       <c r="I116" s="9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J116" s="9"/>
       <c r="K116" s="9" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L116" s="11"/>
       <c r="M116" s="1"/>
@@ -6879,7 +6869,7 @@
       <c r="A117" s="15"/>
       <c r="B117" s="8"/>
       <c r="C117" s="9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D117" s="8"/>
       <c r="E117" s="9"/>
@@ -6887,11 +6877,11 @@
       <c r="G117" s="9"/>
       <c r="H117" s="9"/>
       <c r="I117" s="9" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J117" s="9"/>
       <c r="K117" s="9" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L117" s="11"/>
       <c r="M117" s="1"/>
@@ -7026,7 +7016,7 @@
     </row>
     <row r="121" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B121" s="5"/>
       <c r="C121" s="4"/>
@@ -7337,7 +7327,7 @@
       <c r="B128" s="7"/>
       <c r="C128" s="8"/>
       <c r="D128" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E128" s="9"/>
       <c r="F128" s="9"/>
@@ -7380,7 +7370,7 @@
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D129" s="9"/>
       <c r="E129" s="9"/>
@@ -7392,7 +7382,7 @@
       </c>
       <c r="J129" s="8"/>
       <c r="K129" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L129" s="10"/>
       <c r="M129" s="1"/>
@@ -7436,7 +7426,7 @@
       </c>
       <c r="J130" s="9"/>
       <c r="K130" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L130" s="10"/>
       <c r="M130" s="1"/>
@@ -7482,10 +7472,10 @@
         <v>204</v>
       </c>
       <c r="K131" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L131" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M131" s="1"/>
       <c r="N131" s="1"/>
@@ -7517,7 +7507,7 @@
       <c r="B132" s="7"/>
       <c r="C132" s="8"/>
       <c r="D132" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E132" s="9"/>
       <c r="F132" s="9"/>
@@ -7526,7 +7516,7 @@
       <c r="I132" s="9"/>
       <c r="J132" s="9"/>
       <c r="K132" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L132" s="10"/>
       <c r="M132" s="1"/>
@@ -7559,7 +7549,7 @@
       <c r="B133" s="7"/>
       <c r="C133" s="8"/>
       <c r="D133" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E133" s="9"/>
       <c r="F133" s="9"/>
@@ -7568,7 +7558,7 @@
       <c r="I133" s="9"/>
       <c r="J133" s="9"/>
       <c r="K133" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L133" s="10"/>
       <c r="M133" s="1"/>
@@ -7606,14 +7596,14 @@
       <c r="G134" s="9"/>
       <c r="H134" s="9"/>
       <c r="I134" s="9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J134" s="9"/>
       <c r="K134" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="L134" s="10" t="s">
         <v>317</v>
-      </c>
-      <c r="L134" s="10" t="s">
-        <v>318</v>
       </c>
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
@@ -7650,14 +7640,14 @@
       <c r="G135" s="9"/>
       <c r="H135" s="9"/>
       <c r="I135" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J135" s="9"/>
       <c r="K135" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="L135" s="10" t="s">
         <v>315</v>
-      </c>
-      <c r="L135" s="10" t="s">
-        <v>316</v>
       </c>
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
@@ -7694,14 +7684,14 @@
       <c r="G136" s="9"/>
       <c r="H136" s="9"/>
       <c r="I136" s="9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="J136" s="9"/>
       <c r="K136" s="9" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="L136" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="M136" s="1"/>
       <c r="N136" s="1"/>
@@ -7738,14 +7728,14 @@
       <c r="G137" s="9"/>
       <c r="H137" s="9"/>
       <c r="I137" s="9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J137" s="9"/>
       <c r="K137" s="9" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="L137" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M137" s="1"/>
       <c r="N137" s="1"/>
@@ -7777,7 +7767,7 @@
       <c r="B138" s="7"/>
       <c r="C138" s="8"/>
       <c r="D138" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E138" s="9"/>
       <c r="F138" s="9"/>
@@ -7786,7 +7776,7 @@
       <c r="I138" s="9"/>
       <c r="J138" s="9"/>
       <c r="K138" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L138" s="10"/>
       <c r="M138" s="1"/>
@@ -7819,7 +7809,7 @@
       <c r="B139" s="7"/>
       <c r="C139" s="8"/>
       <c r="D139" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E139" s="9"/>
       <c r="F139" s="9"/>
@@ -7828,10 +7818,10 @@
       <c r="I139" s="9"/>
       <c r="J139" s="9"/>
       <c r="K139" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L139" s="10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
@@ -7863,7 +7853,7 @@
       <c r="B140" s="7"/>
       <c r="C140" s="8"/>
       <c r="D140" s="9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E140" s="9"/>
       <c r="F140" s="9"/>
@@ -7872,10 +7862,10 @@
       <c r="I140" s="9"/>
       <c r="J140" s="9"/>
       <c r="K140" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L140" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="M140" s="1"/>
       <c r="N140" s="1"/>
@@ -7907,7 +7897,7 @@
       <c r="B141" s="7"/>
       <c r="C141" s="8"/>
       <c r="D141" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E141" s="9"/>
       <c r="F141" s="9"/>
@@ -7916,7 +7906,7 @@
       <c r="I141" s="9"/>
       <c r="J141" s="9"/>
       <c r="K141" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L141" s="10"/>
       <c r="M141" s="1"/>
@@ -7949,7 +7939,7 @@
       <c r="B142" s="7"/>
       <c r="C142" s="8"/>
       <c r="D142" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E142" s="9"/>
       <c r="F142" s="9"/>
@@ -7958,7 +7948,7 @@
       <c r="I142" s="9"/>
       <c r="J142" s="9"/>
       <c r="K142" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L142" s="10"/>
       <c r="M142" s="1"/>
@@ -7991,7 +7981,7 @@
       <c r="B143" s="7"/>
       <c r="C143" s="8"/>
       <c r="D143" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E143" s="9"/>
       <c r="F143" s="9"/>
@@ -8000,7 +7990,7 @@
       <c r="I143" s="9"/>
       <c r="J143" s="9"/>
       <c r="K143" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L143" s="10"/>
       <c r="M143" s="1"/>
@@ -8033,7 +8023,7 @@
       <c r="B144" s="7"/>
       <c r="C144" s="8"/>
       <c r="D144" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E144" s="9"/>
       <c r="F144" s="9"/>
@@ -8042,7 +8032,7 @@
       <c r="I144" s="9"/>
       <c r="J144" s="9"/>
       <c r="K144" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L144" s="11"/>
       <c r="M144" s="1"/>
@@ -8079,17 +8069,17 @@
       <c r="F145" s="9"/>
       <c r="G145" s="9"/>
       <c r="H145" s="9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I145" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J145" s="9"/>
       <c r="K145" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L145" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
@@ -8126,16 +8116,16 @@
       <c r="G146" s="9"/>
       <c r="H146" s="9"/>
       <c r="I146" s="9" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J146" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K146" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L146" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M146" s="1"/>
       <c r="N146" s="1"/>
@@ -8165,7 +8155,7 @@
     <row r="147" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="7"/>
       <c r="B147" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C147" s="8" t="s">
         <v>111</v>
@@ -8183,7 +8173,7 @@
         <v>156</v>
       </c>
       <c r="L147" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
@@ -8213,7 +8203,7 @@
     <row r="148" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A148" s="7"/>
       <c r="B148" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C148" s="8"/>
       <c r="D148" s="9" t="s">
@@ -8231,7 +8221,7 @@
         <v>178</v>
       </c>
       <c r="L148" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
@@ -8261,7 +8251,7 @@
     <row r="149" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="7"/>
       <c r="B149" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C149" s="8" t="s">
         <v>112</v>
@@ -8279,7 +8269,7 @@
         <v>157</v>
       </c>
       <c r="L149" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M149" s="1"/>
       <c r="N149" s="1"/>
@@ -8325,7 +8315,7 @@
         <v>158</v>
       </c>
       <c r="L150" s="14" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
@@ -8355,7 +8345,7 @@
     <row r="151" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A151" s="7"/>
       <c r="B151" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C151" s="8"/>
       <c r="D151" s="5"/>
@@ -8364,11 +8354,11 @@
       <c r="G151" s="9"/>
       <c r="H151" s="9"/>
       <c r="I151" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="J151" s="9"/>
       <c r="K151" s="9" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L151" s="10"/>
       <c r="M151" s="1"/>
@@ -8400,7 +8390,7 @@
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="8" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D152" s="9"/>
       <c r="E152" s="9"/>
@@ -8410,10 +8400,10 @@
       <c r="I152" s="9"/>
       <c r="J152" s="9"/>
       <c r="K152" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="L152" s="10" t="s">
         <v>407</v>
-      </c>
-      <c r="L152" s="10" t="s">
-        <v>409</v>
       </c>
       <c r="M152" s="1"/>
       <c r="N152" s="1"/>
@@ -8572,7 +8562,7 @@
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="8" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D160" s="9"/>
       <c r="E160" s="9"/>
@@ -8580,11 +8570,11 @@
       <c r="G160" s="9"/>
       <c r="H160" s="9"/>
       <c r="I160" s="9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J160" s="9"/>
       <c r="K160" s="9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L160" s="10"/>
     </row>
@@ -8592,7 +8582,7 @@
       <c r="A161" s="7"/>
       <c r="B161" s="7"/>
       <c r="C161" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D161" s="9"/>
       <c r="E161" s="9"/>
@@ -8602,10 +8592,10 @@
       <c r="I161" s="9"/>
       <c r="J161" s="9"/>
       <c r="K161" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L161" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.25">
@@ -8632,7 +8622,7 @@
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D163" s="9"/>
       <c r="E163" s="9"/>
@@ -8640,11 +8630,11 @@
       <c r="G163" s="9"/>
       <c r="H163" s="9"/>
       <c r="I163" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J163" s="9"/>
       <c r="K163" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L163" s="10"/>
     </row>

</xml_diff>